<commit_message>
another pack of new scripts
</commit_message>
<xml_diff>
--- a/queries/maintenance/sp/Blitz/sp_AskBrent-CheckID-List.xlsx
+++ b/queries/maintenance/sp/Blitz/sp_AskBrent-CheckID-List.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26101"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brent/Dropbox (Brent Ozar Unlimited)/Projects/sp_AskBrent/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35040" windowHeight="23400"/>
   </bookViews>
   <sheets>
     <sheet name="sp_AskBrent Checks" sheetId="3" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
   <si>
     <t>CheckID</t>
   </si>
@@ -174,9 +179,6 @@
     <t>Database Count</t>
   </si>
   <si>
-    <t>sp_AskBrent Check ID List - v14 2015-03-01</t>
-  </si>
-  <si>
     <t>CPU Utilization</t>
   </si>
   <si>
@@ -184,6 +186,15 @@
   </si>
   <si>
     <t>http://BrentOzar.com/go/cpu</t>
+  </si>
+  <si>
+    <t>Re-Compiles per Second</t>
+  </si>
+  <si>
+    <t>SQL Compilations/sec</t>
+  </si>
+  <si>
+    <t>sp_AskBrent Check ID List - v16 2015-07-18</t>
   </si>
 </sst>
 </file>
@@ -257,7 +268,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="28">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -265,6 +276,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -306,7 +318,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="28">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -332,6 +344,7 @@
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,16 +646,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.1640625" style="4" bestFit="1" customWidth="1"/>
@@ -652,12 +665,12 @@
     <col min="6" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20" thickBot="1">
+    <row r="1" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickTop="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
@@ -665,7 +678,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1">
+    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -682,7 +695,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -699,7 +712,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -716,7 +729,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -733,7 +746,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -750,7 +763,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -767,7 +780,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -784,7 +797,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -801,7 +814,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -818,7 +831,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -835,7 +848,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -852,7 +865,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>11</v>
       </c>
@@ -869,7 +882,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>12</v>
       </c>
@@ -886,7 +899,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>13</v>
       </c>
@@ -903,7 +916,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>14</v>
       </c>
@@ -920,7 +933,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>15</v>
       </c>
@@ -937,7 +950,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>16</v>
       </c>
@@ -954,7 +967,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>17</v>
       </c>
@@ -971,7 +984,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>18</v>
       </c>
@@ -988,7 +1001,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>19</v>
       </c>
@@ -1005,7 +1018,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>20</v>
       </c>
@@ -1022,7 +1035,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>21</v>
       </c>
@@ -1036,7 +1049,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>22</v>
       </c>
@@ -1050,7 +1063,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>23</v>
       </c>
@@ -1061,10 +1074,10 @@
         <v>44</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>24</v>
       </c>
@@ -1075,10 +1088,44 @@
         <v>24</v>
       </c>
       <c r="D28" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="5" t="s">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>25</v>
+      </c>
+      <c r="B29" s="4">
+        <v>250</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>26</v>
+      </c>
+      <c r="B30" s="4">
+        <v>250</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>54</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1107,13 +1154,10 @@
     <hyperlink ref="E23" r:id="rId19"/>
     <hyperlink ref="E28" r:id="rId20"/>
     <hyperlink ref="E24" r:id="rId21"/>
+    <hyperlink ref="E29" r:id="rId22"/>
+    <hyperlink ref="E30" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>